<commit_message>
added nopd rtcc requests data for 3/2022 - 11/2022
</commit_message>
<xml_diff>
--- a/data/excel/armed_robbery_rtcc_footage_request_by_illegal_posses.xlsx
+++ b/data/excel/armed_robbery_rtcc_footage_request_by_illegal_posses.xlsx
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.9266094420600859</v>
+        <v>0.9146688338073954</v>
       </c>
     </row>
     <row r="3">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.07339055793991417</v>
+        <v>0.08533116619260463</v>
       </c>
     </row>
     <row r="4">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2159</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="5">
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>171</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.9791666666666666</v>
+        <v>0.977491961414791</v>
       </c>
     </row>
     <row r="7">
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.022508038585209</v>
       </c>
     </row>
     <row r="8">
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>282</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>